<commit_message>
Update BOM - fix some broken links (Mouser) of ICs - Replace U5 - Passive components untouched
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
+++ b/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Documents\Workspaces\Git\n64rgb\advancedRGBmod\Main-PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\Git\N64RGB\advancedRGBmod\Main-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA6A0C84-1B61-4230-ABA8-AE9384622DB5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_N64_Advanced" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="172">
   <si>
     <t>Designator</t>
   </si>
@@ -119,9 +120,6 @@
     <t>SC-70-6</t>
   </si>
   <si>
-    <t>http://www.mouser.de/ProductDetail/STMicroelectronics/TSH122ICT/</t>
-  </si>
-  <si>
     <t>8-LSSOP, 8-MSOP</t>
   </si>
   <si>
@@ -182,9 +180,6 @@
     <t>https://www.digikey.de/product-detail/de/texas-instruments/TLV70012DDCR/296-39275-1-ND/</t>
   </si>
   <si>
-    <t>http://www.mouser.de/ProductDetail/Texas-Instruments/TLV70012DDCR/</t>
-  </si>
-  <si>
     <t>TLV70025DDCR</t>
   </si>
   <si>
@@ -194,9 +189,6 @@
     <t>https://www.digikey.de/product-detail/de/texas-instruments/TLV70025DDCR/296-32411-1-ND/</t>
   </si>
   <si>
-    <t>http://www.mouser.de/ProductDetail/Texas-Instruments/TLV70025DDCR/</t>
-  </si>
-  <si>
     <t xml:space="preserve">ASE-50.000MHZ-LC-T </t>
   </si>
   <si>
@@ -215,9 +207,6 @@
     <t>https://www.digikey.de/product-detail/de/abracon-llc/ASE-50.000MHZ-LC-T/535-9577-1-ND/</t>
   </si>
   <si>
-    <t>http://www.mouser.de/ProductDetail/ABRACON/ASE-50000MHZ-L-C-T/</t>
-  </si>
-  <si>
     <t>C1,C2</t>
   </si>
   <si>
@@ -428,9 +417,6 @@
     <t>can be replaced with ADV7123KSTZ140 on demand</t>
   </si>
   <si>
-    <t>www.mouser.de/ProductDetail/Analog-Devices/ADV7125KSTZ140/</t>
-  </si>
-  <si>
     <t>https://www.digikey.de/product-detail/de/analog-devices-inc/ADV7125KSTZ140/ADV7125KSTZ140-ND/654207</t>
   </si>
   <si>
@@ -443,12 +429,6 @@
     <t>S25FL116K0XMFB013</t>
   </si>
   <si>
-    <t>http://www.mouser.de/ProductDetail/Cypress/S25FL116K0XMFB013/</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/product-detail/de/cypress-semiconductor-corp/S25FL116K0XMFA043/428-4061-1-ND/</t>
-  </si>
-  <si>
     <t>208mil Body; Digikey ist Alternative im 150mil Body. Footprint ünterstützt beides</t>
   </si>
   <si>
@@ -458,12 +438,6 @@
     <t>10CL010YE144C8G</t>
   </si>
   <si>
-    <t>https://www.digikey.de/product-detail/en/altera/10CL010YE144I7G/544-3376-ND/7347620</t>
-  </si>
-  <si>
-    <t>http://www.mouser.de/ProductDetail/Intel/10CL010YE144C8G/</t>
-  </si>
-  <si>
     <t>Cyclone 10 LP FPGA, 10k LE</t>
   </si>
   <si>
@@ -479,9 +453,6 @@
     <t>TI: DCT Package Footprint</t>
   </si>
   <si>
-    <t>http://www.mouser.de/ProductDetail/Texas-Instruments/SN74LVC3G17DCTR/</t>
-  </si>
-  <si>
     <t>https://www.digikey.de/product-detail/de/texas-instruments/SN74LVC3G17DCTR/296-16915-1-ND/644203</t>
   </si>
   <si>
@@ -540,12 +511,48 @@
   </si>
   <si>
     <t xml:space="preserve">RC0603FR-07523RL </t>
+  </si>
+  <si>
+    <t>IS25LP016D-JBLE-TR</t>
+  </si>
+  <si>
+    <t>208mil Body</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/870-IS25LP016DJBLETR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/issi-integrated-silicon-solution-inc/IS25LP016D-JBLE-TR/706-1599-1-ND/7672068</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/intel-fpgas-altera/10CL010YE144I7G/544-3376-ND/7347620</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Intel-Altera/10CL010YE144C8G?qs=sGAEpiMZZMve4%2fbfQkoj%252bJcIphhECn2a0iFKbSrOfJk%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Analog-Devices/ADV7125KSTZ140?qs=%2fha2pyFaduglq3Ok9Webti7aCr03ycmo%2f90b9HDi8B%2fjL6WBxH3bGA%3d%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/STMicroelectronics/TSH122ICT?qs=%2fha2pyFaduigxW0dT%2fgI7nvf9O5CA4lyihj5iCt%2fxhY%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/SN74LVC3G17DCTR?qs=sGAEpiMZZMuiiWkaIwCK2RZ8fpIXhw4IHpqSVvnkvuY%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TLV70012DDCR?qs=sGAEpiMZZMsGz1a6aV8DcFnW8%252bX0rdBC2IduztBAJN4%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TLV70025DDCR?qs=sGAEpiMZZMsGz1a6aV8DcCniYaGUA430fOrmgOH3ksU%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/ABRACON/ASE-50000MHZ-L-C-T?qs=%2fha2pyFaduiJXabh5egm1N76js19RDbbd6bevDP%252bnxvNwEFIULtJfwJQd%2f%252bio1%252bk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1361,10 +1368,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1408,13 +1417,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -1423,10 +1432,10 @@
         <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1434,7 +1443,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1446,13 +1455,13 @@
         <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1472,10 +1481,10 @@
         <v>28</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>29</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1483,157 +1492,157 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>46</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>47</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>50</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="I8" s="1" t="s">
-        <v>54</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
         <v>55</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>56</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>61</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1642,50 +1651,50 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" t="s">
         <v>64</v>
       </c>
-      <c r="E11" t="s">
+      <c r="H11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="I11" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1694,19 +1703,19 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
         <v>64</v>
       </c>
-      <c r="E13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="H13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1720,19 +1729,19 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1746,88 +1755,88 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B16" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1835,106 +1844,106 @@
         <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="F20" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G21" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1948,129 +1957,129 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F23" t="s">
-        <v>68</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="I23" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="I24" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="F24" t="s">
-        <v>68</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F25" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C26">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2081,61 +2090,56 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="http://www.digikey.de/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=234870402"/>
-    <hyperlink ref="I2" r:id="rId2"/>
-    <hyperlink ref="H3" r:id="rId3"/>
-    <hyperlink ref="I3" r:id="rId4"/>
-    <hyperlink ref="I4" r:id="rId5"/>
-    <hyperlink ref="H4" r:id="rId6"/>
-    <hyperlink ref="I5" r:id="rId7"/>
-    <hyperlink ref="I10" r:id="rId8"/>
-    <hyperlink ref="H10" r:id="rId9"/>
-    <hyperlink ref="H12" r:id="rId10"/>
-    <hyperlink ref="I12" r:id="rId11"/>
-    <hyperlink ref="I6" r:id="rId12"/>
-    <hyperlink ref="H7" r:id="rId13"/>
-    <hyperlink ref="I7" r:id="rId14"/>
-    <hyperlink ref="H8" r:id="rId15"/>
-    <hyperlink ref="I8" r:id="rId16"/>
-    <hyperlink ref="H9" r:id="rId17"/>
-    <hyperlink ref="I9" r:id="rId18"/>
-    <hyperlink ref="H11" r:id="rId19"/>
-    <hyperlink ref="I11" r:id="rId20"/>
-    <hyperlink ref="I13" r:id="rId21"/>
-    <hyperlink ref="H13" r:id="rId22"/>
-    <hyperlink ref="I17" r:id="rId23"/>
-    <hyperlink ref="H14" r:id="rId24"/>
-    <hyperlink ref="I14" r:id="rId25"/>
-    <hyperlink ref="I15" r:id="rId26"/>
-    <hyperlink ref="H15" r:id="rId27"/>
-    <hyperlink ref="H20" r:id="rId28"/>
-    <hyperlink ref="I20" r:id="rId29"/>
-    <hyperlink ref="H19" r:id="rId30"/>
-    <hyperlink ref="I19" r:id="rId31"/>
-    <hyperlink ref="H22" r:id="rId32"/>
-    <hyperlink ref="I22" r:id="rId33"/>
-    <hyperlink ref="I23" r:id="rId34"/>
-    <hyperlink ref="H23" r:id="rId35"/>
-    <hyperlink ref="I24" r:id="rId36"/>
-    <hyperlink ref="H24" r:id="rId37"/>
-    <hyperlink ref="H26" r:id="rId38"/>
-    <hyperlink ref="I26" r:id="rId39"/>
-    <hyperlink ref="I18" r:id="rId40"/>
-    <hyperlink ref="H18" r:id="rId41"/>
-    <hyperlink ref="H21" r:id="rId42"/>
-    <hyperlink ref="I25" r:id="rId43"/>
-    <hyperlink ref="H25" r:id="rId44"/>
-    <hyperlink ref="I27" r:id="rId45"/>
-    <hyperlink ref="H27" r:id="rId46"/>
-    <hyperlink ref="I21" r:id="rId47"/>
-    <hyperlink ref="H6" r:id="rId48"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="I11" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="I13" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="H13" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="I17" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="H14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="I14" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="I15" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="H15" r:id="rId21" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H20" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="I20" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H19" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="I19" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="H22" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="I22" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="I23" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="H23" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="I24" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="H24" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="H26" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="I26" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="I18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="H18" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="H21" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="I25" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="H25" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="I27" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="H27" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="I21" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="H6" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="H5" r:id="rId43" xr:uid="{6749C714-DD08-45FD-BCEA-EA30E9DCFB69}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2176,13 +2180,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -2198,7 +2202,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2210,7 +2214,7 @@
         <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2239,133 +2243,133 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>46</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>48</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
         <v>55</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>56</v>
-      </c>
-      <c r="E8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" t="s">
-        <v>59</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -2374,13 +2378,13 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" t="s">
         <v>64</v>
-      </c>
-      <c r="E11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" t="s">
-        <v>68</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -2396,13 +2400,13 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -2418,123 +2422,123 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G17" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F18" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2550,85 +2554,85 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="1"/>
@@ -2645,7 +2649,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2683,29 +2687,29 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -2714,42 +2718,42 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
         <v>64</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" t="s">
-        <v>68</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2758,13 +2762,13 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
         <v>64</v>
-      </c>
-      <c r="E5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" t="s">
-        <v>68</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2774,85 +2778,85 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -2869,7 +2873,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2907,16 +2911,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>

</xml_diff>

<commit_message>
Recommendation! Replace input resistors by ferrit beads iff one has resistors at RCP output
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
+++ b/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\Git\N64RGB\advancedRGBmod\Main-PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Documents\Workspaces\Git\n64rgb\advancedRGBmod\Main-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA6A0C84-1B61-4230-ABA8-AE9384622DB5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_N64_Advanced" sheetId="1" r:id="rId1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="185">
   <si>
     <t>Designator</t>
   </si>
@@ -396,21 +395,9 @@
     <t>https://www.digikey.de/product-detail/de/bourns-inc/CAT16-47R0F4LF/CAT16-47R0F4LFCT-ND/</t>
   </si>
   <si>
-    <t xml:space="preserve">Alternative: CAY16-47R0F4LF </t>
-  </si>
-  <si>
-    <t>CAT16-47R0F4LF</t>
-  </si>
-  <si>
-    <t>CAT16-75R0F4LF</t>
-  </si>
-  <si>
     <t>https://www.digikey.de/product-detail/de/bourns-inc/CAT16-750J4LF/CAT16-750J4LFCT-ND/</t>
   </si>
   <si>
-    <t>Alternative: CAY16-75R0F4LF; Digi-Key Link zur J4LF Serie (5% Toleranz statt 1%)</t>
-  </si>
-  <si>
     <t>ADV7125KSTZ140</t>
   </si>
   <si>
@@ -547,13 +534,97 @@
   </si>
   <si>
     <t>https://www.mouser.de/ProductDetail/ABRACON/ASE-50000MHZ-L-C-T?qs=%2fha2pyFaduiJXabh5egm1N76js19RDbbd6bevDP%252bnxvNwEFIULtJfwJQd%2f%252bio1%252bk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1761-42R </t>
+  </si>
+  <si>
+    <t>GND Finger</t>
+  </si>
+  <si>
+    <t>GND shield finger</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>3,0mm x 4,5mm pad</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/855-S1761-42R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/harwin-inc/S1761-42R/952-1479-1-ND/2264565</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BK32164M121-T </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ferrite Beads MULTILYR CHP </t>
+  </si>
+  <si>
+    <t>BD 120OHMS 25%</t>
+  </si>
+  <si>
+    <t>Use this if you have resistors at the RCP output</t>
+  </si>
+  <si>
+    <t>CAT16-47R0F4LF / CAY16-47R0F4LF</t>
+  </si>
+  <si>
+    <t>Digi-Key Link zur J4LF Serie (5% Toleranz statt 1%)</t>
+  </si>
+  <si>
+    <t>CAT16-75R0F4LF / CAY16-75R0F4LF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/taiyo-yuden/bk32164m121-t/</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/taiyo-yuden/BK32164M121-T/587-2689-1-ND/2417276</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Only use this if you </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">don't </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>have resistors at the RCP output</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -692,6 +763,15 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1039,7 +1119,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1047,6 +1127,14 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1368,11 +1456,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,13 +1505,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -1432,10 +1520,10 @@
         <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1443,7 +1531,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1455,13 +1543,13 @@
         <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1484,7 +1572,7 @@
         <v>36</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1492,25 +1580,25 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1518,25 +1606,25 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F6" t="s">
         <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1559,7 +1647,7 @@
         <v>48</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1582,7 +1670,7 @@
         <v>51</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1611,7 +1699,7 @@
         <v>57</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1772,10 +1860,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -1784,16 +1872,16 @@
         <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F16" t="s">
         <v>64</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1833,7 +1921,7 @@
         <v>112</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>110</v>
@@ -1867,7 +1955,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
         <v>87</v>
@@ -1896,7 +1984,7 @@
         <v>92</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1905,19 +1993,19 @@
         <v>83</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F21" t="s">
         <v>64</v>
       </c>
       <c r="G21" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2024,125 +2112,179 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>130</v>
-      </c>
-      <c r="B26" t="s">
-        <v>122</v>
-      </c>
-      <c r="C26">
+    <row r="26" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C26" s="8">
         <v>3</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" t="s">
+        <v>181</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="H26" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>129</v>
-      </c>
-      <c r="B27" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27">
+      <c r="I28" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30">
         <v>2</v>
       </c>
-      <c r="D27" t="s">
-        <v>104</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F27" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
+      <c r="D30" t="s">
+        <v>170</v>
+      </c>
+      <c r="F30" t="s">
+        <v>172</v>
+      </c>
+      <c r="G30" t="s">
+        <v>171</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
     </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="I10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="H12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="I12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="H7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="H8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="H9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="H11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="I11" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="I13" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="H13" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="I17" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="H14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="I14" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="I15" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="H15" r:id="rId21" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="H20" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="I20" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="H19" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="I19" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="H22" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="I22" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="I23" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="H23" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="I24" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="H24" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="H26" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="I26" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="I18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="H18" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="H21" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="I25" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="H25" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="I27" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="H27" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="I21" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="H6" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="H5" r:id="rId43" xr:uid="{6749C714-DD08-45FD-BCEA-EA30E9DCFB69}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="I3" r:id="rId4"/>
+    <hyperlink ref="H4" r:id="rId5"/>
+    <hyperlink ref="I10" r:id="rId6"/>
+    <hyperlink ref="H10" r:id="rId7"/>
+    <hyperlink ref="H12" r:id="rId8"/>
+    <hyperlink ref="I12" r:id="rId9"/>
+    <hyperlink ref="H7" r:id="rId10"/>
+    <hyperlink ref="H8" r:id="rId11"/>
+    <hyperlink ref="H9" r:id="rId12"/>
+    <hyperlink ref="H11" r:id="rId13"/>
+    <hyperlink ref="I11" r:id="rId14"/>
+    <hyperlink ref="I13" r:id="rId15"/>
+    <hyperlink ref="H13" r:id="rId16"/>
+    <hyperlink ref="I17" r:id="rId17"/>
+    <hyperlink ref="H14" r:id="rId18"/>
+    <hyperlink ref="I14" r:id="rId19"/>
+    <hyperlink ref="I15" r:id="rId20"/>
+    <hyperlink ref="H15" r:id="rId21"/>
+    <hyperlink ref="H20" r:id="rId22"/>
+    <hyperlink ref="I20" r:id="rId23"/>
+    <hyperlink ref="H19" r:id="rId24"/>
+    <hyperlink ref="I19" r:id="rId25"/>
+    <hyperlink ref="H22" r:id="rId26"/>
+    <hyperlink ref="I22" r:id="rId27"/>
+    <hyperlink ref="I23" r:id="rId28"/>
+    <hyperlink ref="H23" r:id="rId29"/>
+    <hyperlink ref="I24" r:id="rId30"/>
+    <hyperlink ref="H24" r:id="rId31"/>
+    <hyperlink ref="H26" r:id="rId32"/>
+    <hyperlink ref="I26" r:id="rId33"/>
+    <hyperlink ref="I18" r:id="rId34"/>
+    <hyperlink ref="H18" r:id="rId35"/>
+    <hyperlink ref="H21" r:id="rId36"/>
+    <hyperlink ref="I25" r:id="rId37"/>
+    <hyperlink ref="H25" r:id="rId38"/>
+    <hyperlink ref="I28" r:id="rId39"/>
+    <hyperlink ref="H28" r:id="rId40"/>
+    <hyperlink ref="I21" r:id="rId41"/>
+    <hyperlink ref="H6" r:id="rId42"/>
+    <hyperlink ref="H5" r:id="rId43"/>
+    <hyperlink ref="I30" r:id="rId44"/>
+    <hyperlink ref="H30" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId46"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H20:I24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2180,13 +2322,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -2202,7 +2344,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2214,7 +2356,7 @@
         <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2243,19 +2385,19 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2347,7 +2489,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
         <v>116</v>
@@ -2369,7 +2511,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -2435,10 +2577,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -2447,7 +2589,7 @@
         <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F14" t="s">
         <v>64</v>
@@ -2476,7 +2618,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B16" t="s">
         <v>87</v>
@@ -2501,7 +2643,7 @@
         <v>92</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2510,20 +2652,20 @@
         <v>83</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F17" t="s">
         <v>64</v>
       </c>
       <c r="G17" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>96</v>
@@ -2587,55 +2729,74 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21">
+    <row r="21" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" s="8">
         <v>3</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>129</v>
-      </c>
-      <c r="B22" t="s">
-        <v>123</v>
-      </c>
-      <c r="C22">
+      <c r="G21" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23">
         <v>2</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H22" s="4"/>
-      <c r="I22" s="1"/>
+      <c r="G23" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
@@ -2649,10 +2810,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2690,19 +2853,19 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F2" t="s">
         <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2731,7 +2894,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
         <v>116</v>
@@ -2753,7 +2916,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2797,7 +2960,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
         <v>87</v>
@@ -2819,7 +2982,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>96</v>
@@ -2860,6 +3023,26 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>170</v>
+      </c>
+      <c r="F11" t="s">
+        <v>172</v>
+      </c>
+      <c r="G11" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
@@ -2873,7 +3056,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>